<commit_message>
Stopped exceptions when reading String in Excel
</commit_message>
<xml_diff>
--- a/Test/UnitTest/srcTest/dataframe.xlsx
+++ b/Test/UnitTest/srcTest/dataframe.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
   <si>
     <t>dron</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>col3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -112,11 +118,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -724,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,8 +749,8 @@
       </c>
     </row>
     <row r="2" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D2">
-        <v>1</v>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -756,8 +763,8 @@
       <c r="D3">
         <v>3</v>
       </c>
-      <c r="E3">
-        <v>4</v>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="F3">
         <v>5.0999999999999996</v>
@@ -783,7 +790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Add simple Insert data private all other add simple data
</commit_message>
<xml_diff>
--- a/Test/UnitTest/srcTest/dataframe.xlsx
+++ b/Test/UnitTest/srcTest/dataframe.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
@@ -17,78 +17,97 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
-  <si>
-    <t>dron</t>
-  </si>
-  <si>
-    <t>header</t>
-  </si>
-  <si>
-    <t>sdds</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>asdas</t>
-  </si>
-  <si>
-    <t>rrg</t>
-  </si>
-  <si>
-    <t>g4</t>
-  </si>
-  <si>
-    <t>wer</t>
-  </si>
-  <si>
-    <t>a1</t>
-  </si>
-  <si>
-    <t>a2</t>
-  </si>
-  <si>
-    <t>a3</t>
-  </si>
-  <si>
-    <t>a4</t>
-  </si>
-  <si>
-    <t>a7</t>
-  </si>
-  <si>
-    <t>ыуаа</t>
-  </si>
-  <si>
-    <t>ыва</t>
-  </si>
-  <si>
-    <t>ывапр</t>
-  </si>
-  <si>
-    <t>р</t>
-  </si>
-  <si>
-    <t>col1</t>
-  </si>
-  <si>
-    <t>col2</t>
-  </si>
-  <si>
-    <t>col3</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>4</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="28">
+  <si>
+    <t xml:space="preserve">dron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rrg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ыуаа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ыва</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ывапр</t>
+  </si>
+  <si>
+    <t xml:space="preserve">р</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2r3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3we</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wer1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3wer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34wr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -116,7 +135,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -131,11 +150,11 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -364,7 +383,7 @@
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
-          <a:sp3d>
+          <a:sp3d prstMaterial="warmMatte">
             <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
@@ -427,7 +446,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -541,13 +560,211 @@
         <v>asdaswer</v>
       </c>
     </row>
+    <row r="16">
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="F24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="F25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="F26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="F32" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" t="s">
+        <v>23</v>
+      </c>
+      <c r="H32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="F33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="F34" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" t="s">
+        <v>26</v>
+      </c>
+      <c r="H34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="F40" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" t="s">
+        <v>23</v>
+      </c>
+      <c r="H40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="F41" t="s">
+        <v>20</v>
+      </c>
+      <c r="G41" t="s">
+        <v>24</v>
+      </c>
+      <c r="H41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="F42" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" t="s">
+        <v>26</v>
+      </c>
+      <c r="H42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -728,7 +945,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="D1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -787,7 +1004,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:AI13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>